<commit_message>
add novas analises fem-masc
diferenca entre homens e mulhere
</commit_message>
<xml_diff>
--- a/correlacao_completa.xlsx
+++ b/correlacao_completa.xlsx
@@ -31,22 +31,22 @@
     <t>mesesNoProjeto</t>
   </si>
   <si>
-    <t>Burnout_cinismo</t>
-  </si>
-  <si>
-    <t>Burnout_exaustao</t>
-  </si>
-  <si>
-    <t>Burnout_eficacia</t>
-  </si>
-  <si>
-    <t>instabilidade_equipe</t>
-  </si>
-  <si>
-    <t>instabilidade_tecnica</t>
-  </si>
-  <si>
-    <t>instabilidade_tarefa</t>
+    <t>Cinismo</t>
+  </si>
+  <si>
+    <t>Exaustão</t>
+  </si>
+  <si>
+    <t>Eficacia</t>
+  </si>
+  <si>
+    <t>Inst.Equipe</t>
+  </si>
+  <si>
+    <t>Inst.Tecnica</t>
+  </si>
+  <si>
+    <t>Inst.Tarefa</t>
   </si>
 </sst>
 </file>

</xml_diff>